<commit_message>
bug in job card
</commit_message>
<xml_diff>
--- a/application/controllers/BookingJobCard_Template-v6.xlsx
+++ b/application/controllers/BookingJobCard_Template-v6.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/aroundlocalhost/application/controllers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/247around-adminp-dev/application/controllers/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -205,17 +205,14 @@
     </r>
   </si>
   <si>
-    <t>{booking:total}</t>
-  </si>
-  <si>
-    <t>{booking:final}</t>
+    <t>{booking:amount}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -267,6 +264,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -773,7 +778,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -907,6 +912,90 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="22" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -916,91 +1005,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="22" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1400,7 +1408,7 @@
   <dimension ref="B2:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:G14"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1427,12 +1435,12 @@
     <row r="4" spans="2:12" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5"/>
       <c r="C4" s="6"/>
-      <c r="D4" s="59" t="s">
+      <c r="D4" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="60"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="72"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
@@ -1442,17 +1450,17 @@
       <c r="B5" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="56"/>
+      <c r="D5" s="57"/>
       <c r="E5" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="53" t="s">
+      <c r="F5" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="54" t="s">
+      <c r="G5" s="68" t="s">
         <v>25</v>
       </c>
       <c r="I5" s="6"/>
@@ -1461,19 +1469,19 @@
       <c r="L5" s="6"/>
     </row>
     <row r="6" spans="2:12" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="63" t="s">
+      <c r="C6" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="64" t="s">
+      <c r="D6" s="48" t="s">
         <v>28</v>
       </c>
       <c r="E6" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="50" t="s">
+      <c r="F6" s="51" t="s">
         <v>34</v>
       </c>
       <c r="G6" s="52"/>
@@ -1483,17 +1491,17 @@
       <c r="L6" s="6"/>
     </row>
     <row r="7" spans="2:12" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="62"/>
-      <c r="C7" s="65" t="s">
+      <c r="B7" s="46"/>
+      <c r="C7" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="66" t="s">
+      <c r="D7" s="50" t="s">
         <v>28</v>
       </c>
       <c r="E7" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="50" t="s">
+      <c r="F7" s="51" t="s">
         <v>42</v>
       </c>
       <c r="G7" s="52" t="s">
@@ -1508,16 +1516,16 @@
       <c r="B8" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="57" t="s">
+      <c r="C8" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="58" t="s">
+      <c r="D8" s="70" t="s">
         <v>27</v>
       </c>
       <c r="E8" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="50" t="s">
+      <c r="F8" s="51" t="s">
         <v>43</v>
       </c>
       <c r="G8" s="52" t="s">
@@ -1538,10 +1546,10 @@
       <c r="D9" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="69" t="s">
+      <c r="E9" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="70"/>
+      <c r="F9" s="60"/>
       <c r="G9" s="26" t="s">
         <v>50</v>
       </c>
@@ -1550,7 +1558,7 @@
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
     </row>
-    <row r="10" spans="2:12" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
         <v>39</v>
       </c>
@@ -1560,10 +1568,10 @@
       <c r="D10" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="E10" s="71" t="s">
+      <c r="E10" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="72"/>
+      <c r="F10" s="62"/>
       <c r="G10" s="12" t="s">
         <v>35</v>
       </c>
@@ -1576,29 +1584,30 @@
       <c r="B11" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="73" t="s">
+      <c r="C11" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="74"/>
-      <c r="E11" s="75" t="s">
+      <c r="D11" s="64"/>
+      <c r="E11" s="65" t="s">
         <v>53</v>
       </c>
       <c r="F11" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="15" t="s">
-        <v>54</v>
+      <c r="G11" s="77" t="e">
+        <f>G12+G13</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="12" spans="2:12" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="55" t="s">
+      <c r="C12" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="68"/>
-      <c r="E12" s="75"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="65"/>
       <c r="F12" s="29" t="s">
         <v>48</v>
       </c>
@@ -1610,35 +1619,35 @@
       <c r="B13" s="21"/>
       <c r="C13" s="8"/>
       <c r="D13" s="13"/>
-      <c r="E13" s="76"/>
+      <c r="E13" s="66"/>
       <c r="F13" s="29" t="s">
         <v>49</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="2:12" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="50" t="s">
+      <c r="C14" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="76"/>
       <c r="G14" s="52"/>
     </row>
     <row r="15" spans="2:12" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="67"/>
-      <c r="D15" s="68"/>
-      <c r="E15" s="68"/>
-      <c r="F15" s="68"/>
-      <c r="G15" s="56"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="57"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B16" s="30" t="s">
@@ -1694,8 +1703,8 @@
       <c r="B20" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="48"/>
-      <c r="D20" s="49"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="54"/>
       <c r="E20" s="18"/>
       <c r="F20" s="36" t="s">
         <v>9</v>
@@ -1706,8 +1715,8 @@
       <c r="B21" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="48"/>
-      <c r="D21" s="49"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="54"/>
       <c r="E21" s="18"/>
       <c r="F21" s="36" t="s">
         <v>10</v>
@@ -1718,8 +1727,8 @@
       <c r="B22" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="48"/>
-      <c r="D22" s="49"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="54"/>
       <c r="E22" s="18"/>
       <c r="F22" s="37" t="s">
         <v>11</v>
@@ -1730,8 +1739,8 @@
       <c r="B23" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="48"/>
-      <c r="D23" s="49"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="54"/>
       <c r="E23" s="18"/>
       <c r="F23" s="36" t="s">
         <v>12</v>
@@ -1749,14 +1758,14 @@
       <c r="G24" s="20"/>
     </row>
     <row r="25" spans="2:7" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="45" t="s">
+      <c r="B25" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="C25" s="46"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="46"/>
-      <c r="F25" s="46"/>
-      <c r="G25" s="47"/>
+      <c r="C25" s="74"/>
+      <c r="D25" s="74"/>
+      <c r="E25" s="74"/>
+      <c r="F25" s="74"/>
+      <c r="G25" s="75"/>
     </row>
     <row r="26" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="41"/>
@@ -1770,6 +1779,16 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="D4:G4"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:D7"/>
     <mergeCell ref="F8:G8"/>
@@ -1781,16 +1800,6 @@
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="E11:E13"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C14:G14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>